<commit_message>
fixed frame rate entry
</commit_message>
<xml_diff>
--- a/tests/excel_optical_data/optical_data_filled_template.xlsx
+++ b/tests/excel_optical_data/optical_data_filled_template.xlsx
@@ -62,9 +62,6 @@
     <t>Do twitches point upward? (y/n)</t>
   </si>
   <si>
-    <t>Sampling Period / Frame rate of camera (in seconds)</t>
-  </si>
-  <si>
     <t>Timestamp of when recording began (use YYYY-MM-DD HH:MM format)</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Interpolation Value (In seconds) (This will resample data at a new period. If left blank, data will not be interpolated)</t>
+  </si>
+  <si>
+    <t>Sampling Rate / Frame rate of camera (in Hz)</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:F1467"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -543,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -572,7 +572,7 @@
         <v>44116.194444444445</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -583,7 +583,7 @@
         <v>3.1063370187234698</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>5</v>
@@ -597,10 +597,10 @@
         <v>3.2629563416485299</v>
       </c>
       <c r="E5" s="11">
-        <v>1.6666E-2</v>
+        <v>60</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -625,10 +625,10 @@
         <v>0.67211373356121795</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -642,7 +642,7 @@
         <v>1.23E-2</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>